<commit_message>
Obtendo dados e transformando em excel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,37 +1,244 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
+  <si>
+    <t>imgCapa</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Titulo</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>ano</t>
+  </si>
+  <si>
+    <t>Paginas</t>
+  </si>
+  <si>
+    <t>Preço</t>
+  </si>
+  <si>
+    <t>Estoque</t>
+  </si>
+  <si>
+    <t>pgAutores.pgAutor1</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>pgLivro</t>
+  </si>
+  <si>
+    <t>autores.autor2</t>
+  </si>
+  <si>
+    <t>pgAutores.pgAutor2</t>
+  </si>
+  <si>
+    <t>https://s3.novatec.com.br/capas/9788575226834.jpg</t>
+  </si>
+  <si>
+    <t>https://s3.novatec.com.br/capas/9788575226674.jpg</t>
+  </si>
+  <si>
+    <t>https://s3.novatec.com.br/capas/9788575226681.jpg</t>
+  </si>
+  <si>
+    <t>https://s3.novatec.com.br/capas/9788575226568.jpg</t>
+  </si>
+  <si>
+    <t>https://s3.novatec.com.br/capas/9788575225905.jpg</t>
+  </si>
+  <si>
+    <t>https://s3.novatec.com.br/capas/9788575225462.jpg</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Morbi eleifend, purus quis laoreet faucibus, ante augue malesuada mi, id rhoncus augue lorem eget elit. Ut sollicitudin sodales purus.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Phasellus libero felis, blandit nec, commodo ut, imperdiet ut, nibh. Suspendisse potenti. Donec ullamcorper cursus dolor. Duis vitae ipsum. Maecenas dapibus hendrerit diam. Morbi varius, massa id pretium accumsan, nunc lorem congue libero, ut euismod metus libero id nulla.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Duis posuere odio sed velit vulputate venenatis. Suspendisse et dui ac metus auctor fringilla. Curabitur interdum augue a pede.&lt;/p&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Duis cursus, dui non dictum tincidunt, wisi ipsum mollis wisi, nec ornare velit ipsum eget enim. In sed felis. Phasellus condimentum sodales nulla. Etiam orci leo, rutrum malesuada, congue vel, fringilla vitae, lorem. Pellentesque ligula.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Cras gravida. Mauris consequat aliquam leo. Aenean non tortor id metus aliquet consectetuer. Quisque sodales lectus ac orci. Donec eleifend fringilla mi. Vivamus vel massa. Aenean interdum pellentesque sem. Nulla pellentesque felis et tortor. Duis cursus, dui non dictum tincidunt, wisi ipsum mollis wisi, nec ornare velit ipsum eget enim. In sed felis. Phasellus condimentum sodales nulla. Etiam orci leo, rutrum malesuada, congue vel, fringilla vitae, lorem. Pellentesque ligula.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Morbi eleifend, purus quis laoreet faucibus, ante augue malesuada mi, id rhoncus augue lorem eget elit. Ut sollicitudin sodales purus. Phasellus libero felis, blandit nec, commodo ut, imperdiet ut, nibh. Suspendisse potenti. Donec ullamcorper cursus dolor. Duis vitae ipsum. Maecenas dapibus hendrerit diam. Morbi varius, massa id pretium accumsan, nunc lorem congue libero, ut euismod metus libero id nulla. Duis posuere odio sed velit vulputate venenatis. Suspendisse et dui ac metus auctor fringilla. Curabitur interdum augue a pede.&lt;/p&gt;&lt;p&gt;Curabitur hendrerit erat ut augue. Cras gravida. Mauris consequat aliquam leo. Aenean non tortor id metus aliquet consectetuer. Quisque sodales lectus ac orci. Donec eleifend fringilla mi. Vivamus vel massa. Aenean interdum pellentesque sem. Nulla pellentesque felis et tortor. Duis cursus, dui non dictum tincidunt, wisi ipsum mollis wisi, nec ornare velit ipsum eget enim. In sed felis. Phasellus condimentum sodales nulla. Etiam orci leo, rutrum malesuada, congue vel, fringilla vitae, lorem. Pellentesque ligula.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Primeiros passos com a linguagem Rust</t>
+  </si>
+  <si>
+    <t>ProgramaÃ§Ã£o em Baixo NÃ­vel</t>
+  </si>
+  <si>
+    <t>IntroduÃ§Ã£o Ã  linguagem Lua</t>
+  </si>
+  <si>
+    <t>LÃ³gica de ProgramaÃ§Ã£o e Algoritmos com JavaScript</t>
+  </si>
+  <si>
+    <t>PHP para quem conhece PHP - 5Âª EdiÃ§Ã£o</t>
+  </si>
+  <si>
+    <t>A Linguagem de ProgramaÃ§Ã£o Go</t>
+  </si>
+  <si>
+    <t>ProgramaÃ§Ã£o</t>
+  </si>
+  <si>
+    <t>Hardware &amp;amp; RobÃ³tica</t>
+  </si>
+  <si>
+    <t>978-85-7522-683-4</t>
+  </si>
+  <si>
+    <t>978-85-7522-667-4</t>
+  </si>
+  <si>
+    <t>978-85-7522-668-1</t>
+  </si>
+  <si>
+    <t>978-85-7522-656-8</t>
+  </si>
+  <si>
+    <t>978-85-7522-590-5</t>
+  </si>
+  <si>
+    <t>978-85-7522-546-2</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>312</t>
+  </si>
+  <si>
+    <t>576</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>544</t>
+  </si>
+  <si>
+    <t>480</t>
+  </si>
+  <si>
+    <t>DisponÃ­vel tambÃ©m em formato ebook</t>
+  </si>
+  <si>
+    <t>autores/jose-manzano.php</t>
+  </si>
+  <si>
+    <t>autores/igor-zhirkov.php</t>
+  </si>
+  <si>
+    <t>autores/edecio-iepsen.php</t>
+  </si>
+  <si>
+    <t>autores/niederauer.php</t>
+  </si>
+  <si>
+    <t>autores/alan-donovan.php</t>
+  </si>
+  <si>
+    <t>JosÃ© Augusto N. G. Manzano</t>
+  </si>
+  <si>
+    <t>Igor Zhirkov</t>
+  </si>
+  <si>
+    <t>EdÃ©cio Fernando Iepsen</t>
+  </si>
+  <si>
+    <t>Juliano Niederauer</t>
+  </si>
+  <si>
+    <t>Alan A. Donovan</t>
+  </si>
+  <si>
+    <t>livros/introducao-a-linguagem-lua</t>
+  </si>
+  <si>
+    <t>livros/php-para-quem-conhece-php-5ed/</t>
+  </si>
+  <si>
+    <t>livros/linguagem-de-programacao-go/</t>
+  </si>
+  <si>
+    <t>Brian W. Kernighan</t>
+  </si>
+  <si>
+    <t>autores/brian-kernighan.php</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +253,41 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,87 +575,306 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>livros</t>
-        </is>
+    <row r="1" spans="1:15">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:15">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>{'imgCapa': 'https://s3.novatec.com.br/capas/9788575226834.jpg', 'descricao': '&lt;p&gt;Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Morbi eleifend, purus quis laoreet faucibus, ante augue malesuada mi, id rhoncus augue lorem eget elit. Ut sollicitudin sodales purus.&lt;/p&gt;', 'titulo': 'Primeiros passos com a linguagem Rust', 'pgAutores': {'pgAutor1': 'autores/jose-manzano.php'}, 'autores': {'autor1': 'José Augusto N. G. Manzano'}, 'categoria': 'Programação', 'isbn': '978-85-7522-683-4', 'ano': '2018', 'paginas': '312', 'preco': 69, 'estoque': 'Disponível também em formato ebook'}</t>
-        </is>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:15">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>{'imgCapa': 'https://s3.novatec.com.br/capas/9788575226674.jpg', 'descricao': '&lt;p&gt;Phasellus libero felis, blandit nec, commodo ut, imperdiet ut, nibh. Suspendisse potenti. Donec ullamcorper cursus dolor. Duis vitae ipsum. Maecenas dapibus hendrerit diam. Morbi varius, massa id pretium accumsan, nunc lorem congue libero, ut euismod metus libero id nulla.&lt;/p&gt;', 'titulo': 'Programação em Baixo Nível', 'pgAutores': {'pgAutor1': 'autores/igor-zhirkov.php'}, 'autores': {'autor1': 'Igor Zhirkov'}, 'categoria': 'Hardware &amp;amp; Robótica', 'isbn': '978-85-7522-667-4', 'ano': '2018', 'paginas': '576', 'preco': 120, 'estoque': 'Disponível também em formato ebook'}</t>
-        </is>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3">
+        <v>120</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:15">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>{'imgCapa': 'https://s3.novatec.com.br/capas/9788575226681.jpg', 'pgLivro': 'livros/introducao-a-linguagem-lua', 'descricao': '&lt;p&gt;Duis posuere odio sed velit vulputate venenatis. Suspendisse et dui ac metus auctor fringilla. Curabitur interdum augue a pede.&lt;/p&gt;&gt;', 'titulo': 'Introdução à linguagem Lua', 'pgAutores': {'pgAutor1': 'autores/jose-manzano.php'}, 'autores': {'autor1': 'José Augusto N. G. Manzano'}, 'categoria': 'Programação', 'isbn': '978-85-7522-668-1', 'ano': '2018', 'paginas': '176', 'preco': 52, 'estoque': 'Disponível também em formato ebook'}</t>
-        </is>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4">
+        <v>52</v>
+      </c>
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:15">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>{'imgCapa': 'https://s3.novatec.com.br/capas/9788575226568.jpg', 'descricao': '&lt;p&gt;Duis cursus, dui non dictum tincidunt, wisi ipsum mollis wisi, nec ornare velit ipsum eget enim. In sed felis. Phasellus condimentum sodales nulla. Etiam orci leo, rutrum malesuada, congue vel, fringilla vitae, lorem. Pellentesque ligula.&lt;/p&gt;', 'titulo': 'Lógica de Programação e Algoritmos com JavaScript', 'pgAutores': {'pgAutor1': 'autores/edecio-iepsen.php'}, 'autores': {'autor1': 'Edécio Fernando Iepsen'}, 'categoria': 'Programação', 'isbn': '978-85-7522-656-8', 'ano': '2018', 'paginas': '320', 'preco': 69, 'estoque': 'Disponível também em formato ebook'}</t>
-        </is>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5">
+        <v>69</v>
+      </c>
+      <c r="J5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:15">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>{'imgCapa': 'https://s3.novatec.com.br/capas/9788575225905.jpg', 'pgLivro': 'livros/php-para-quem-conhece-php-5ed/', 'descricao': '&lt;p&gt;Cras gravida. Mauris consequat aliquam leo. Aenean non tortor id metus aliquet consectetuer. Quisque sodales lectus ac orci. Donec eleifend fringilla mi. Vivamus vel massa. Aenean interdum pellentesque sem. Nulla pellentesque felis et tortor. Duis cursus, dui non dictum tincidunt, wisi ipsum mollis wisi, nec ornare velit ipsum eget enim. In sed felis. Phasellus condimentum sodales nulla. Etiam orci leo, rutrum malesuada, congue vel, fringilla vitae, lorem. Pellentesque ligula.&lt;/p&gt;', 'titulo': 'PHP para quem conhece PHP - 5ª Edição', 'pgAutores': {'pgAutor1': 'autores/niederauer.php'}, 'autores': {'autor1': 'Juliano Niederauer'}, 'categoria': 'Programação', 'isbn': '978-85-7522-590-5', 'ano': '2017', 'paginas': '544', 'preco': 99, 'estoque': 'Disponível também em formato ebook'}</t>
-        </is>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6">
+        <v>99</v>
+      </c>
+      <c r="J6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M6" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:15">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>{'imgCapa': 'https://s3.novatec.com.br/capas/9788575225462.jpg', 'pgLivro': 'livros/linguagem-de-programacao-go/', 'descricao': '&lt;p&gt;Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Morbi eleifend, purus quis laoreet faucibus, ante augue malesuada mi, id rhoncus augue lorem eget elit. Ut sollicitudin sodales purus. Phasellus libero felis, blandit nec, commodo ut, imperdiet ut, nibh. Suspendisse potenti. Donec ullamcorper cursus dolor. Duis vitae ipsum. Maecenas dapibus hendrerit diam. Morbi varius, massa id pretium accumsan, nunc lorem congue libero, ut euismod metus libero id nulla. Duis posuere odio sed velit vulputate venenatis. Suspendisse et dui ac metus auctor fringilla. Curabitur interdum augue a pede.&lt;/p&gt;&lt;p&gt;Curabitur hendrerit erat ut augue. Cras gravida. Mauris consequat aliquam leo. Aenean non tortor id metus aliquet consectetuer. Quisque sodales lectus ac orci. Donec eleifend fringilla mi. Vivamus vel massa. Aenean interdum pellentesque sem. Nulla pellentesque felis et tortor. Duis cursus, dui non dictum tincidunt, wisi ipsum mollis wisi, nec ornare velit ipsum eget enim. In sed felis. Phasellus condimentum sodales nulla. Etiam orci leo, rutrum malesuada, congue vel, fringilla vitae, lorem. Pellentesque ligula.&lt;/p&gt;', 'titulo': 'A Linguagem de Programação Go', 'autores': {'autor1': 'Alan A. Donovan', 'autor2': 'Brian W. Kernighan'}, 'pgAutores': {'pgAutor1': 'autores/alan-donovan.php', 'pgAutor2': 'autores/brian-kernighan.php'}, 'categoria': 'Programação', 'isbn': '978-85-7522-546-2', 'ano': '2017', 'paginas': '480', 'preco': 98, 'estoque': ''}</t>
-        </is>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7">
+        <v>98</v>
+      </c>
+      <c r="K7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>